<commit_message>
My progress so far in MVP functions
</commit_message>
<xml_diff>
--- a/Project0/DataSpreadsheet/Client.xlsx
+++ b/Project0/DataSpreadsheet/Client.xlsx
@@ -16,21 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>bread</t>
+    <t>Client0</t>
   </si>
   <si>
-    <t>milk</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>eggs</t>
+    <t>ShoppingList</t>
   </si>
   <si>
-    <t>fruit</t>
-  </si>
-  <si>
-    <t>Client0</t>
+    <t>Bread, Eggs, Milk, Apples, Oranges, Cucumber</t>
   </si>
 </sst>
 </file>
@@ -369,37 +366,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <pane ySplit="2700" topLeftCell="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>